<commit_message>
Added Version 2's for editing
</commit_message>
<xml_diff>
--- a/SPSWENG_SystemScape_GroupEstimationWorksheet_v1.xlsx
+++ b/SPSWENG_SystemScape_GroupEstimationWorksheet_v1.xlsx
@@ -1019,22 +1019,26 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFCC4125"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1051,7 +1055,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1064,17 +1068,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1261,11 +1254,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1274,13 +1308,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1292,88 +1326,96 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1677,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:I8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8:U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1772,19 +1814,19 @@
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
@@ -1793,13 +1835,13 @@
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1812,109 +1854,109 @@
     <row r="7" spans="1:21" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="35" t="s">
+      <c r="B8" s="32"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="22" t="s">
         <v>328</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="24" t="s">
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="25"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="39" t="s">
+      <c r="K8" s="32"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="25" t="s">
         <v>328</v>
       </c>
-      <c r="N8" s="40"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="38" t="s">
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="R8" s="24" t="s">
+      <c r="R8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="S8" s="25"/>
-      <c r="T8" s="26"/>
-      <c r="U8" s="30" t="s">
+      <c r="S8" s="32"/>
+      <c r="T8" s="33"/>
+      <c r="U8" s="44" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="33" t="s">
+      <c r="A9" s="34"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="27"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="33" t="s">
+      <c r="J9" s="34"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="34" t="s">
+      <c r="N9" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="O9" s="34" t="s">
+      <c r="O9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="34" t="s">
+      <c r="P9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="29"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="36"/>
+      <c r="U9" s="45"/>
     </row>
     <row r="10" spans="1:21" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21">
+      <c r="A10" s="15">
         <v>1</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="17" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -1929,17 +1971,17 @@
       <c r="H10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="15">
         <v>1</v>
       </c>
-      <c r="K10" s="22" t="s">
+      <c r="K10" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="23"/>
-      <c r="M10" s="20" t="s">
+      <c r="L10" s="36"/>
+      <c r="M10" s="14" t="s">
         <v>26</v>
       </c>
       <c r="N10" s="5" t="s">
@@ -1951,29 +1993,29 @@
       <c r="P10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="Q10" s="5" t="s">
+      <c r="Q10" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="R10" s="21">
+      <c r="R10" s="15">
         <v>1</v>
       </c>
-      <c r="S10" s="18" t="s">
+      <c r="S10" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="T10" s="19"/>
-      <c r="U10" s="31" t="s">
+      <c r="T10" s="28"/>
+      <c r="U10" s="43" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16">
+      <c r="A11" s="12">
         <v>2</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="17" t="s">
+      <c r="C11" s="28"/>
+      <c r="D11" s="13" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -1991,14 +2033,14 @@
       <c r="I11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="16">
+      <c r="J11" s="12">
         <v>2</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="19"/>
-      <c r="M11" s="17" t="s">
+      <c r="L11" s="28"/>
+      <c r="M11" s="13" t="s">
         <v>39</v>
       </c>
       <c r="N11" s="5" t="s">
@@ -2013,26 +2055,26 @@
       <c r="Q11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="R11" s="16">
+      <c r="R11" s="12">
         <v>2</v>
       </c>
-      <c r="S11" s="18" t="s">
+      <c r="S11" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="T11" s="19"/>
-      <c r="U11" s="31" t="s">
+      <c r="T11" s="28"/>
+      <c r="U11" s="16" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
+      <c r="A12" s="12">
         <v>3</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="17" t="s">
+      <c r="C12" s="28"/>
+      <c r="D12" s="13" t="s">
         <v>46</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -2050,14 +2092,14 @@
       <c r="I12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12" s="12">
         <v>3</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="L12" s="19"/>
-      <c r="M12" s="17" t="s">
+      <c r="L12" s="28"/>
+      <c r="M12" s="13" t="s">
         <v>52</v>
       </c>
       <c r="N12" s="5" t="s">
@@ -2072,26 +2114,26 @@
       <c r="Q12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="R12" s="16">
+      <c r="R12" s="12">
         <v>3</v>
       </c>
-      <c r="S12" s="18" t="s">
+      <c r="S12" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="T12" s="19"/>
-      <c r="U12" s="31" t="s">
+      <c r="T12" s="28"/>
+      <c r="U12" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16">
+      <c r="A13" s="12">
         <v>4</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="17" t="s">
+      <c r="C13" s="28"/>
+      <c r="D13" s="13" t="s">
         <v>59</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -2109,14 +2151,14 @@
       <c r="I13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13" s="12">
         <v>4</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="K13" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="L13" s="19"/>
-      <c r="M13" s="17" t="s">
+      <c r="L13" s="28"/>
+      <c r="M13" s="13" t="s">
         <v>65</v>
       </c>
       <c r="N13" s="5" t="s">
@@ -2131,26 +2173,26 @@
       <c r="Q13" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="R13" s="16">
+      <c r="R13" s="12">
         <v>4</v>
       </c>
-      <c r="S13" s="18" t="s">
+      <c r="S13" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="T13" s="19"/>
-      <c r="U13" s="31" t="s">
+      <c r="T13" s="28"/>
+      <c r="U13" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16">
+      <c r="A14" s="12">
         <v>5</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="17" t="s">
+      <c r="C14" s="28"/>
+      <c r="D14" s="13" t="s">
         <v>72</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -2168,14 +2210,14 @@
       <c r="I14" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="J14" s="16">
+      <c r="J14" s="12">
         <v>5</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="K14" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="L14" s="19"/>
-      <c r="M14" s="17" t="s">
+      <c r="L14" s="28"/>
+      <c r="M14" s="13" t="s">
         <v>78</v>
       </c>
       <c r="N14" s="5" t="s">
@@ -2190,26 +2232,26 @@
       <c r="Q14" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="R14" s="16">
+      <c r="R14" s="12">
         <v>5</v>
       </c>
-      <c r="S14" s="18" t="s">
+      <c r="S14" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="T14" s="19"/>
-      <c r="U14" s="31" t="s">
+      <c r="T14" s="28"/>
+      <c r="U14" s="16" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16">
+      <c r="A15" s="12">
         <v>6</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="17" t="s">
+      <c r="C15" s="28"/>
+      <c r="D15" s="13" t="s">
         <v>85</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -2227,14 +2269,14 @@
       <c r="I15" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J15" s="12">
         <v>6</v>
       </c>
-      <c r="K15" s="18" t="s">
+      <c r="K15" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="L15" s="19"/>
-      <c r="M15" s="17" t="s">
+      <c r="L15" s="28"/>
+      <c r="M15" s="13" t="s">
         <v>91</v>
       </c>
       <c r="N15" s="5" t="s">
@@ -2249,26 +2291,26 @@
       <c r="Q15" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="R15" s="16">
+      <c r="R15" s="12">
         <v>6</v>
       </c>
-      <c r="S15" s="18" t="s">
+      <c r="S15" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="T15" s="19"/>
-      <c r="U15" s="31" t="s">
+      <c r="T15" s="28"/>
+      <c r="U15" s="16" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16">
+      <c r="A16" s="12">
         <v>7</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="17" t="s">
+      <c r="C16" s="28"/>
+      <c r="D16" s="13" t="s">
         <v>98</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -2286,14 +2328,14 @@
       <c r="I16" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="J16" s="16">
+      <c r="J16" s="12">
         <v>7</v>
       </c>
-      <c r="K16" s="18" t="s">
+      <c r="K16" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="L16" s="19"/>
-      <c r="M16" s="17" t="s">
+      <c r="L16" s="28"/>
+      <c r="M16" s="13" t="s">
         <v>104</v>
       </c>
       <c r="N16" s="5" t="s">
@@ -2308,26 +2350,26 @@
       <c r="Q16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="R16" s="16">
+      <c r="R16" s="12">
         <v>7</v>
       </c>
-      <c r="S16" s="18" t="s">
+      <c r="S16" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="T16" s="19"/>
-      <c r="U16" s="31" t="s">
+      <c r="T16" s="28"/>
+      <c r="U16" s="16" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16">
+      <c r="A17" s="12">
         <v>8</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="17" t="s">
+      <c r="C17" s="28"/>
+      <c r="D17" s="13" t="s">
         <v>111</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -2345,14 +2387,14 @@
       <c r="I17" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="J17" s="16">
+      <c r="J17" s="12">
         <v>8</v>
       </c>
-      <c r="K17" s="18" t="s">
+      <c r="K17" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="L17" s="19"/>
-      <c r="M17" s="17" t="s">
+      <c r="L17" s="28"/>
+      <c r="M17" s="13" t="s">
         <v>117</v>
       </c>
       <c r="N17" s="5" t="s">
@@ -2367,26 +2409,26 @@
       <c r="Q17" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="R17" s="16">
+      <c r="R17" s="12">
         <v>8</v>
       </c>
-      <c r="S17" s="18" t="s">
+      <c r="S17" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="T17" s="19"/>
-      <c r="U17" s="31" t="s">
+      <c r="T17" s="28"/>
+      <c r="U17" s="16" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16">
+      <c r="A18" s="12">
         <v>9</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="17" t="s">
+      <c r="C18" s="28"/>
+      <c r="D18" s="13" t="s">
         <v>124</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -2404,14 +2446,14 @@
       <c r="I18" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="J18" s="16">
+      <c r="J18" s="12">
         <v>9</v>
       </c>
-      <c r="K18" s="18" t="s">
+      <c r="K18" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="L18" s="19"/>
-      <c r="M18" s="17" t="s">
+      <c r="L18" s="28"/>
+      <c r="M18" s="13" t="s">
         <v>130</v>
       </c>
       <c r="N18" s="5" t="s">
@@ -2426,26 +2468,26 @@
       <c r="Q18" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="R18" s="16">
+      <c r="R18" s="12">
         <v>9</v>
       </c>
-      <c r="S18" s="18" t="s">
+      <c r="S18" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="T18" s="19"/>
-      <c r="U18" s="31" t="s">
+      <c r="T18" s="28"/>
+      <c r="U18" s="16" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16">
+      <c r="A19" s="12">
         <v>10</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="17" t="s">
+      <c r="C19" s="28"/>
+      <c r="D19" s="13" t="s">
         <v>137</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -2463,14 +2505,14 @@
       <c r="I19" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="J19" s="16">
+      <c r="J19" s="12">
         <v>10</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="K19" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="L19" s="19"/>
-      <c r="M19" s="17" t="s">
+      <c r="L19" s="28"/>
+      <c r="M19" s="13" t="s">
         <v>143</v>
       </c>
       <c r="N19" s="5" t="s">
@@ -2485,26 +2527,26 @@
       <c r="Q19" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="R19" s="16">
+      <c r="R19" s="12">
         <v>10</v>
       </c>
-      <c r="S19" s="18" t="s">
+      <c r="S19" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="T19" s="19"/>
-      <c r="U19" s="31" t="s">
+      <c r="T19" s="28"/>
+      <c r="U19" s="16" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16">
+      <c r="A20" s="12">
         <v>11</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="17" t="s">
+      <c r="C20" s="28"/>
+      <c r="D20" s="13" t="s">
         <v>150</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -2522,14 +2564,14 @@
       <c r="I20" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="J20" s="16">
+      <c r="J20" s="12">
         <v>11</v>
       </c>
-      <c r="K20" s="18" t="s">
+      <c r="K20" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="L20" s="19"/>
-      <c r="M20" s="17" t="s">
+      <c r="L20" s="28"/>
+      <c r="M20" s="13" t="s">
         <v>156</v>
       </c>
       <c r="N20" s="5" t="s">
@@ -2544,26 +2586,26 @@
       <c r="Q20" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="R20" s="16">
+      <c r="R20" s="12">
         <v>11</v>
       </c>
-      <c r="S20" s="18" t="s">
+      <c r="S20" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="T20" s="19"/>
-      <c r="U20" s="31" t="s">
+      <c r="T20" s="28"/>
+      <c r="U20" s="16" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16">
+      <c r="A21" s="12">
         <v>12</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="17" t="s">
+      <c r="C21" s="28"/>
+      <c r="D21" s="13" t="s">
         <v>163</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -2581,14 +2623,14 @@
       <c r="I21" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="J21" s="16">
+      <c r="J21" s="12">
         <v>12</v>
       </c>
-      <c r="K21" s="18" t="s">
+      <c r="K21" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="L21" s="19"/>
-      <c r="M21" s="17" t="s">
+      <c r="L21" s="28"/>
+      <c r="M21" s="13" t="s">
         <v>169</v>
       </c>
       <c r="N21" s="5" t="s">
@@ -2603,26 +2645,26 @@
       <c r="Q21" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="R21" s="16">
+      <c r="R21" s="12">
         <v>12</v>
       </c>
-      <c r="S21" s="18" t="s">
+      <c r="S21" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="T21" s="19"/>
-      <c r="U21" s="31" t="s">
+      <c r="T21" s="28"/>
+      <c r="U21" s="16" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="16">
+      <c r="A22" s="12">
         <v>13</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="17" t="s">
+      <c r="C22" s="28"/>
+      <c r="D22" s="13" t="s">
         <v>175</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -2640,14 +2682,14 @@
       <c r="I22" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="J22" s="16">
+      <c r="J22" s="12">
         <v>13</v>
       </c>
-      <c r="K22" s="18" t="s">
+      <c r="K22" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="L22" s="19"/>
-      <c r="M22" s="17" t="s">
+      <c r="L22" s="28"/>
+      <c r="M22" s="13" t="s">
         <v>181</v>
       </c>
       <c r="N22" s="5" t="s">
@@ -2662,26 +2704,26 @@
       <c r="Q22" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="R22" s="16">
+      <c r="R22" s="12">
         <v>13</v>
       </c>
-      <c r="S22" s="18" t="s">
+      <c r="S22" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="T22" s="19"/>
-      <c r="U22" s="31" t="s">
+      <c r="T22" s="28"/>
+      <c r="U22" s="16" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16">
+      <c r="A23" s="12">
         <v>14</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="17" t="s">
+      <c r="C23" s="28"/>
+      <c r="D23" s="13" t="s">
         <v>188</v>
       </c>
       <c r="E23" s="5" t="s">
@@ -2699,14 +2741,14 @@
       <c r="I23" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="J23" s="16">
+      <c r="J23" s="12">
         <v>14</v>
       </c>
-      <c r="K23" s="18" t="s">
+      <c r="K23" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="L23" s="19"/>
-      <c r="M23" s="17" t="s">
+      <c r="L23" s="28"/>
+      <c r="M23" s="13" t="s">
         <v>194</v>
       </c>
       <c r="N23" s="5" t="s">
@@ -2721,26 +2763,26 @@
       <c r="Q23" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="R23" s="16">
+      <c r="R23" s="12">
         <v>14</v>
       </c>
-      <c r="S23" s="18" t="s">
+      <c r="S23" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="T23" s="19"/>
-      <c r="U23" s="31" t="s">
+      <c r="T23" s="28"/>
+      <c r="U23" s="16" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16">
+      <c r="A24" s="12">
         <v>15</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="17" t="s">
+      <c r="C24" s="28"/>
+      <c r="D24" s="13" t="s">
         <v>200</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -2758,14 +2800,14 @@
       <c r="I24" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="J24" s="16">
+      <c r="J24" s="12">
         <v>15</v>
       </c>
-      <c r="K24" s="18" t="s">
+      <c r="K24" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="L24" s="19"/>
-      <c r="M24" s="17" t="s">
+      <c r="L24" s="28"/>
+      <c r="M24" s="13" t="s">
         <v>206</v>
       </c>
       <c r="N24" s="5" t="s">
@@ -2780,26 +2822,26 @@
       <c r="Q24" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="R24" s="16">
+      <c r="R24" s="12">
         <v>15</v>
       </c>
-      <c r="S24" s="18" t="s">
+      <c r="S24" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="T24" s="19"/>
-      <c r="U24" s="31" t="s">
+      <c r="T24" s="28"/>
+      <c r="U24" s="16" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="16">
+      <c r="A25" s="12">
         <v>16</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="17" t="s">
+      <c r="C25" s="28"/>
+      <c r="D25" s="13" t="s">
         <v>213</v>
       </c>
       <c r="E25" s="5" t="s">
@@ -2817,14 +2859,14 @@
       <c r="I25" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="J25" s="16">
+      <c r="J25" s="12">
         <v>16</v>
       </c>
-      <c r="K25" s="18" t="s">
+      <c r="K25" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="L25" s="19"/>
-      <c r="M25" s="17" t="s">
+      <c r="L25" s="28"/>
+      <c r="M25" s="13" t="s">
         <v>219</v>
       </c>
       <c r="N25" s="5" t="s">
@@ -2842,23 +2884,23 @@
       <c r="R25" s="4">
         <v>16</v>
       </c>
-      <c r="S25" s="32" t="s">
+      <c r="S25" s="29" t="s">
         <v>212</v>
       </c>
-      <c r="T25" s="14"/>
+      <c r="T25" s="30"/>
       <c r="U25" s="6" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16">
+      <c r="A26" s="12">
         <v>17</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="17" t="s">
+      <c r="C26" s="28"/>
+      <c r="D26" s="13" t="s">
         <v>226</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -2876,14 +2918,14 @@
       <c r="I26" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="J26" s="16">
+      <c r="J26" s="12">
         <v>17</v>
       </c>
-      <c r="K26" s="18" t="s">
+      <c r="K26" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="L26" s="19"/>
-      <c r="M26" s="17" t="s">
+      <c r="L26" s="28"/>
+      <c r="M26" s="13" t="s">
         <v>232</v>
       </c>
       <c r="N26" s="5" t="s">
@@ -2898,26 +2940,26 @@
       <c r="Q26" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="R26" s="16">
+      <c r="R26" s="12">
         <v>17</v>
       </c>
-      <c r="S26" s="18" t="s">
+      <c r="S26" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="T26" s="19"/>
-      <c r="U26" s="31" t="s">
+      <c r="T26" s="28"/>
+      <c r="U26" s="16" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="16">
+      <c r="A27" s="12">
         <v>18</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="17" t="s">
+      <c r="C27" s="28"/>
+      <c r="D27" s="13" t="s">
         <v>239</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -2935,14 +2977,14 @@
       <c r="I27" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="J27" s="16">
+      <c r="J27" s="12">
         <v>18</v>
       </c>
-      <c r="K27" s="18" t="s">
+      <c r="K27" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="L27" s="19"/>
-      <c r="M27" s="17" t="s">
+      <c r="L27" s="28"/>
+      <c r="M27" s="13" t="s">
         <v>245</v>
       </c>
       <c r="N27" s="5" t="s">
@@ -2957,26 +2999,26 @@
       <c r="Q27" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="R27" s="16">
+      <c r="R27" s="12">
         <v>18</v>
       </c>
-      <c r="S27" s="18" t="s">
+      <c r="S27" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="T27" s="19"/>
-      <c r="U27" s="31" t="s">
+      <c r="T27" s="28"/>
+      <c r="U27" s="16" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="16">
+      <c r="A28" s="12">
         <v>19</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="17" t="s">
+      <c r="C28" s="28"/>
+      <c r="D28" s="13" t="s">
         <v>251</v>
       </c>
       <c r="E28" s="5" t="s">
@@ -2994,14 +3036,14 @@
       <c r="I28" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="J28" s="16">
+      <c r="J28" s="12">
         <v>19</v>
       </c>
-      <c r="K28" s="18" t="s">
+      <c r="K28" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="L28" s="19"/>
-      <c r="M28" s="17" t="s">
+      <c r="L28" s="28"/>
+      <c r="M28" s="13" t="s">
         <v>257</v>
       </c>
       <c r="N28" s="5" t="s">
@@ -3016,26 +3058,26 @@
       <c r="Q28" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="R28" s="16">
+      <c r="R28" s="12">
         <v>19</v>
       </c>
-      <c r="S28" s="18" t="s">
+      <c r="S28" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="T28" s="19"/>
-      <c r="U28" s="31" t="s">
+      <c r="T28" s="28"/>
+      <c r="U28" s="16" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="16">
+      <c r="A29" s="12">
         <v>20</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="27" t="s">
         <v>263</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="17" t="s">
+      <c r="C29" s="28"/>
+      <c r="D29" s="13" t="s">
         <v>264</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -3053,14 +3095,14 @@
       <c r="I29" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="J29" s="16">
+      <c r="J29" s="12">
         <v>20</v>
       </c>
-      <c r="K29" s="18" t="s">
+      <c r="K29" s="27" t="s">
         <v>263</v>
       </c>
-      <c r="L29" s="19"/>
-      <c r="M29" s="17" t="s">
+      <c r="L29" s="28"/>
+      <c r="M29" s="13" t="s">
         <v>270</v>
       </c>
       <c r="N29" s="5" t="s">
@@ -3075,26 +3117,26 @@
       <c r="Q29" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="R29" s="16">
+      <c r="R29" s="12">
         <v>20</v>
       </c>
-      <c r="S29" s="18" t="s">
+      <c r="S29" s="27" t="s">
         <v>263</v>
       </c>
-      <c r="T29" s="19"/>
-      <c r="U29" s="31" t="s">
+      <c r="T29" s="28"/>
+      <c r="U29" s="16" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="16">
+      <c r="A30" s="12">
         <v>21</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="27" t="s">
         <v>275</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="17" t="s">
+      <c r="C30" s="28"/>
+      <c r="D30" s="13" t="s">
         <v>276</v>
       </c>
       <c r="E30" s="5" t="s">
@@ -3112,14 +3154,14 @@
       <c r="I30" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="J30" s="16">
+      <c r="J30" s="12">
         <v>21</v>
       </c>
-      <c r="K30" s="18" t="s">
+      <c r="K30" s="27" t="s">
         <v>275</v>
       </c>
-      <c r="L30" s="19"/>
-      <c r="M30" s="17" t="s">
+      <c r="L30" s="28"/>
+      <c r="M30" s="13" t="s">
         <v>282</v>
       </c>
       <c r="N30" s="5" t="s">
@@ -3134,26 +3176,26 @@
       <c r="Q30" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="R30" s="16">
+      <c r="R30" s="12">
         <v>21</v>
       </c>
-      <c r="S30" s="18" t="s">
+      <c r="S30" s="27" t="s">
         <v>275</v>
       </c>
-      <c r="T30" s="19"/>
-      <c r="U30" s="31" t="s">
+      <c r="T30" s="28"/>
+      <c r="U30" s="16" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="16">
+      <c r="A31" s="12">
         <v>22</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="17" t="s">
+      <c r="C31" s="28"/>
+      <c r="D31" s="13" t="s">
         <v>289</v>
       </c>
       <c r="E31" s="5" t="s">
@@ -3171,14 +3213,14 @@
       <c r="I31" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="J31" s="16">
+      <c r="J31" s="12">
         <v>22</v>
       </c>
-      <c r="K31" s="18" t="s">
+      <c r="K31" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="L31" s="19"/>
-      <c r="M31" s="17" t="s">
+      <c r="L31" s="28"/>
+      <c r="M31" s="13" t="s">
         <v>295</v>
       </c>
       <c r="N31" s="5" t="s">
@@ -3193,26 +3235,26 @@
       <c r="Q31" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="R31" s="16">
+      <c r="R31" s="12">
         <v>22</v>
       </c>
-      <c r="S31" s="18" t="s">
+      <c r="S31" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="T31" s="19"/>
-      <c r="U31" s="31" t="s">
+      <c r="T31" s="28"/>
+      <c r="U31" s="16" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="16">
+      <c r="A32" s="12">
         <v>23</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="27" t="s">
         <v>301</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="17" t="s">
+      <c r="C32" s="28"/>
+      <c r="D32" s="13" t="s">
         <v>302</v>
       </c>
       <c r="E32" s="5" t="s">
@@ -3230,14 +3272,14 @@
       <c r="I32" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="J32" s="16">
+      <c r="J32" s="12">
         <v>23</v>
       </c>
-      <c r="K32" s="18" t="s">
+      <c r="K32" s="27" t="s">
         <v>301</v>
       </c>
-      <c r="L32" s="19"/>
-      <c r="M32" s="17" t="s">
+      <c r="L32" s="28"/>
+      <c r="M32" s="13" t="s">
         <v>308</v>
       </c>
       <c r="N32" s="5" t="s">
@@ -3252,26 +3294,26 @@
       <c r="Q32" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="R32" s="16">
+      <c r="R32" s="12">
         <v>23</v>
       </c>
-      <c r="S32" s="18" t="s">
+      <c r="S32" s="27" t="s">
         <v>301</v>
       </c>
-      <c r="T32" s="19"/>
-      <c r="U32" s="31" t="s">
+      <c r="T32" s="28"/>
+      <c r="U32" s="16" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="16">
+      <c r="A33" s="12">
         <v>24</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="27" t="s">
         <v>313</v>
       </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="17" t="s">
+      <c r="C33" s="28"/>
+      <c r="D33" s="13" t="s">
         <v>314</v>
       </c>
       <c r="E33" s="5" t="s">
@@ -3289,14 +3331,14 @@
       <c r="I33" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="J33" s="16">
+      <c r="J33" s="12">
         <v>24</v>
       </c>
-      <c r="K33" s="18" t="s">
+      <c r="K33" s="27" t="s">
         <v>313</v>
       </c>
-      <c r="L33" s="19"/>
-      <c r="M33" s="17" t="s">
+      <c r="L33" s="28"/>
+      <c r="M33" s="13" t="s">
         <v>320</v>
       </c>
       <c r="N33" s="5" t="s">
@@ -3311,23 +3353,23 @@
       <c r="Q33" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="R33" s="16">
+      <c r="R33" s="12">
         <v>24</v>
       </c>
-      <c r="S33" s="18" t="s">
+      <c r="S33" s="27" t="s">
         <v>313</v>
       </c>
-      <c r="T33" s="19"/>
-      <c r="U33" s="31" t="s">
+      <c r="T33" s="28"/>
+      <c r="U33" s="16" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="19" t="s">
         <v>326</v>
       </c>
-      <c r="C34" s="10"/>
+      <c r="C34" s="20"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
@@ -3335,25 +3377,25 @@
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="7"/>
-      <c r="K34" s="12" t="s">
+      <c r="K34" s="19" t="s">
         <v>326</v>
       </c>
-      <c r="L34" s="10"/>
+      <c r="L34" s="20"/>
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
       <c r="O34" s="9"/>
       <c r="R34" s="7"/>
-      <c r="S34" s="12" t="s">
+      <c r="S34" s="19" t="s">
         <v>326</v>
       </c>
-      <c r="T34" s="10"/>
+      <c r="T34" s="20"/>
     </row>
     <row r="35" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="C35" s="10"/>
+      <c r="C35" s="20"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
@@ -3361,21 +3403,93 @@
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="7"/>
-      <c r="K35" s="12" t="s">
+      <c r="K35" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="L35" s="10"/>
+      <c r="L35" s="20"/>
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
       <c r="O35" s="9"/>
       <c r="R35" s="7"/>
-      <c r="S35" s="12" t="s">
+      <c r="S35" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="T35" s="10"/>
+      <c r="T35" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="86">
+  <mergeCells count="88">
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="C7:K7"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="J8:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="R8:T9"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="S18:T18"/>
     <mergeCell ref="S34:T34"/>
     <mergeCell ref="S35:T35"/>
     <mergeCell ref="C5:G5"/>
@@ -3392,76 +3506,6 @@
     <mergeCell ref="S27:T27"/>
     <mergeCell ref="S28:T28"/>
     <mergeCell ref="S19:T19"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="R8:T9"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="J8:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="C7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>